<commit_message>
Size of book-images reduced
</commit_message>
<xml_diff>
--- a/LIB-LIST.xlsx
+++ b/LIB-LIST.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="387" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="436" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="1" state="visible" r:id="rId2"/>
@@ -6363,14 +6363,14 @@
   </sheetPr>
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A27" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B32" activeCellId="0" pane="topLeft" sqref="B32"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B120" activeCellId="0" pane="topLeft" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.9176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.1803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="1">
@@ -9075,9 +9075,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.7450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.9960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1">
@@ -10318,7 +10318,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="1">
@@ -13597,12 +13597,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.7882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.1490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -16004,7 +16004,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="1">
@@ -16159,9 +16159,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="65.65" outlineLevel="0" r="1">
@@ -16933,15 +16933,15 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6117647058823"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4862745098039"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.9" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Book image files - extension updated
</commit_message>
<xml_diff>
--- a/LIB-LIST.xlsx
+++ b/LIB-LIST.xlsx
@@ -6372,14 +6372,14 @@
   </sheetPr>
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A144" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A144" activeCellId="0" pane="topLeft" sqref="A144"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.443137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.7137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="1">
@@ -9084,9 +9084,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.243137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.4941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1">
@@ -10327,7 +10327,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="1">
@@ -13606,12 +13606,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.121568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.8823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -16013,7 +16013,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="1">
@@ -16168,9 +16168,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="65.65" outlineLevel="0" r="1">
@@ -16947,10 +16947,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.6705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.9" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
isbn codes updated in LIB-LIST.xlsx
</commit_message>
<xml_diff>
--- a/LIB-LIST.xlsx
+++ b/LIB-LIST.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="436" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="436" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="1" state="visible" r:id="rId2"/>
@@ -1684,7 +1684,7 @@
     <t>BILLEGAS EDITORS</t>
   </si>
   <si>
-    <t>958-8156-06-8</t>
+    <t>ISBN 958-8156-06-8</t>
   </si>
   <si>
     <t>B2</t>
@@ -1699,7 +1699,7 @@
     <t>OSCAR HIDALGO LOPEZ EDITORS</t>
   </si>
   <si>
-    <t>958-33-4298-X</t>
+    <t>ISBN 958-33-4298-X</t>
   </si>
   <si>
     <t>B3</t>
@@ -1714,7 +1714,7 @@
     <t>WITRA WESIN MUSEUM</t>
   </si>
   <si>
-    <t>3-931936-25-2</t>
+    <t>ISBN 3-931936-25-2</t>
   </si>
   <si>
     <t>B4</t>
@@ -1741,7 +1741,7 @@
     <t>NATIONAL INSTITUTE OF DESIGN</t>
   </si>
   <si>
-    <t>81-86199-50-0</t>
+    <t>ISBN 81-86199-50-0</t>
   </si>
   <si>
     <t>B7</t>
@@ -1768,7 +1768,7 @@
     <t>TRADA TECHNOLOGY</t>
   </si>
   <si>
-    <t>1-9005-10-03-0</t>
+    <t>ISBN 1-9005-10-03-0</t>
   </si>
   <si>
     <t>B9</t>
@@ -1981,7 +1981,7 @@
     <t>BAM CITY</t>
   </si>
   <si>
-    <t>964-6561-23-3</t>
+    <t>ISBN 964-6561-23-3</t>
   </si>
   <si>
     <t>B35</t>
@@ -2008,7 +2008,7 @@
     <t>GIBBS SMITH PUBLISHER</t>
   </si>
   <si>
-    <t>1-58685-220-5</t>
+    <t>ISBN 1-58685-220-5</t>
   </si>
   <si>
     <t>B37</t>
@@ -2023,7 +2023,7 @@
     <t>SHELTER PUBLICATION</t>
   </si>
   <si>
-    <t>0-963070-33-1</t>
+    <t>ISBN 0-963070-33-1</t>
   </si>
   <si>
     <t>B38</t>
@@ -2287,7 +2287,7 @@
     <t>PRACTICAL ACTION PUBLISHING</t>
   </si>
   <si>
-    <t>978-1-85339-203-0</t>
+    <t>ISBN 978-1-85339-203-0</t>
   </si>
   <si>
     <t>B70</t>
@@ -4129,7 +4129,7 @@
     <t>OXFORD UNIVERSITY</t>
   </si>
   <si>
-    <t>019565632-6</t>
+    <t>ISBN 019565632-6</t>
   </si>
   <si>
     <t>G2</t>
@@ -4153,7 +4153,7 @@
     <t>TTK PHARMA  LTD</t>
   </si>
   <si>
-    <t>81-7053-000-8</t>
+    <t>ISBN 81-7053-000-8</t>
   </si>
   <si>
     <t>G4</t>
@@ -4171,7 +4171,7 @@
     <t>INDIAN MAP SERVICE</t>
   </si>
   <si>
-    <t>81-87460-55-5</t>
+    <t>ISBN 81-87460-55-5</t>
   </si>
   <si>
     <t>G6</t>
@@ -4183,7 +4183,7 @@
     <t>R.P.ARYA</t>
   </si>
   <si>
-    <t>81-87460-05-9</t>
+    <t>ISBN 81-87460-05-9</t>
   </si>
   <si>
     <t>G7</t>
@@ -4192,7 +4192,7 @@
     <t>THE ROAD ATLAS OF INDIA</t>
   </si>
   <si>
-    <t>81-7053-033-4</t>
+    <t>ISBN 81-7053-033-4</t>
   </si>
   <si>
     <t>G8</t>
@@ -4207,7 +4207,7 @@
     <t>TTK HEALTHCARE  LTD</t>
   </si>
   <si>
-    <t>81-7053-022-9</t>
+    <t>ISBN 81-7053-022-9</t>
   </si>
   <si>
     <t>G9</t>
@@ -4216,7 +4216,7 @@
     <t>A ROAD GUIDE TO DELHI WITH MAP</t>
   </si>
   <si>
-    <t>81-7053-020-2</t>
+    <t>ISBN 81-7053-020-2</t>
   </si>
   <si>
     <t>G10</t>
@@ -4234,7 +4234,7 @@
     <t>R P ARYA,JITENDRA ARYA</t>
   </si>
   <si>
-    <t>81-87460-23-7</t>
+    <t>ISBN 81-87460-23-7</t>
   </si>
   <si>
     <t>G12</t>
@@ -4243,7 +4243,7 @@
     <t>MUMBAI - ROAD GUIDE WITH MAP</t>
   </si>
   <si>
-    <t>81-7053-009-1</t>
+    <t>ISBN 81-7053-009-1</t>
   </si>
   <si>
     <t>G13</t>
@@ -4258,7 +4258,7 @@
     <t>A ROAD GUIDE TO CHENNAI</t>
   </si>
   <si>
-    <t>81-7053-129-2</t>
+    <t>ISBN 81-7053-129-2</t>
   </si>
   <si>
     <t>G15</t>
@@ -4267,7 +4267,7 @@
     <t>A ROAD GUIDE TO PONDICHERRY WITH MAP</t>
   </si>
   <si>
-    <t>81-7053-025-3</t>
+    <t>ISBN 81-7053-025-3</t>
   </si>
   <si>
     <t>G16</t>
@@ -4279,7 +4279,7 @@
     <t>I</t>
   </si>
   <si>
-    <t>81-7053-107-1</t>
+    <t>ISBN 81-7053-107-1</t>
   </si>
   <si>
     <t>G17</t>
@@ -4288,7 +4288,7 @@
     <t>A ROAD GUIDE TO ORISSA &amp; MAP</t>
   </si>
   <si>
-    <t>81-7053-085-7</t>
+    <t>ISBN 81-7053-085-7</t>
   </si>
   <si>
     <t>G18</t>
@@ -4297,7 +4297,7 @@
     <t>A ROAD GUIDE TO PUNE &amp; MAP</t>
   </si>
   <si>
-    <t>81-7053-131-4</t>
+    <t>ISBN 81-7053-131-4</t>
   </si>
   <si>
     <t>G19</t>
@@ -4306,7 +4306,7 @@
     <t>A ROAD GUIDE TO M.P &amp; MAP</t>
   </si>
   <si>
-    <t>81-7053-014-8</t>
+    <t>ISBN 81-7053-014-8</t>
   </si>
   <si>
     <t>G20A</t>
@@ -4939,7 +4939,7 @@
     <t>AVA PUBLISHING</t>
   </si>
   <si>
-    <t>2-88479-013-6</t>
+    <t>ISBN 2-88479-013-6</t>
   </si>
   <si>
     <t>G101A</t>
@@ -4957,7 +4957,7 @@
     <t>INSPIRING CREATIVE WEB DESIGN</t>
   </si>
   <si>
-    <t>2-88479-017-9</t>
+    <t>ISBN 2-88479-017-9</t>
   </si>
   <si>
     <t>G102A</t>
@@ -5038,7 +5038,7 @@
     <t>TTK HEALTHCARE LTD</t>
   </si>
   <si>
-    <t>81-7053-143-8</t>
+    <t>ISBN 81-7053-143-8</t>
   </si>
   <si>
     <t>G118</t>
@@ -5056,7 +5056,7 @@
     <t>NIMBY BOOKS</t>
   </si>
   <si>
-    <t>978-93-80658-03-2</t>
+    <t>ISBN 978-93-80658-03-2</t>
   </si>
   <si>
     <t>G120</t>
@@ -6372,14 +6372,12 @@
   </sheetPr>
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A136" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.7137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="1">
@@ -9079,14 +9077,12 @@
   </sheetPr>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A74" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B77" activeCellId="0" pane="topLeft" sqref="B77"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A73" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E75" activeCellId="0" pane="topLeft" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.4941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1">
@@ -10322,13 +10318,10 @@
   </sheetPr>
   <dimension ref="A1:F198"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A197" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E197" activeCellId="0" pane="topLeft" sqref="E197"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E54" activeCellId="0" pane="topLeft" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
-  </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.65" outlineLevel="0" r="1">
       <c r="A1" s="43" t="s">
@@ -13601,17 +13594,15 @@
   </sheetPr>
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A163" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B127" activeCellId="0" pane="topLeft" sqref="B127"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A113" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E124" activeCellId="0" pane="topLeft" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.8823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.7411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.2549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -16012,9 +16003,6 @@
       <selection activeCell="F8" activeCellId="0" pane="topLeft" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
-  </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="1">
       <c r="A1" s="71" t="s">
@@ -16168,9 +16156,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.8823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="65.65" outlineLevel="0" r="1">
@@ -16947,10 +16933,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.321568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.9" outlineLevel="0" r="1">

</xml_diff>